<commit_message>
updated wbs and pop for delivery 2
</commit_message>
<xml_diff>
--- a/wbs-and-pop.xlsx
+++ b/wbs-and-pop.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ander\work\H25\konstruksjon-av-innebygde-systemer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459AFA98-5F0D-4FF4-8554-1B57F46A943A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490E0718-FA40-4B25-8E49-A4D2D819BD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="2" xr2:uid="{88374655-B4FF-47ED-8C62-5C3447431953}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="3" xr2:uid="{88374655-B4FF-47ED-8C62-5C3447431953}"/>
   </bookViews>
   <sheets>
     <sheet name="work-breakdown-structure" sheetId="2" r:id="rId1"/>
     <sheet name="plan-of-progress-initial" sheetId="1" r:id="rId2"/>
-    <sheet name="plan-of-progress-first-update" sheetId="4" r:id="rId3"/>
+    <sheet name="plan-of-progress-1" sheetId="4" r:id="rId3"/>
+    <sheet name="plan-of-progress-2" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="115">
   <si>
     <t>WBS_ID</t>
   </si>
@@ -341,6 +342,45 @@
   </si>
   <si>
     <t>3 | 4</t>
+  </si>
+  <si>
+    <t>Week49</t>
+  </si>
+  <si>
+    <t>Week48</t>
+  </si>
+  <si>
+    <t>Week47</t>
+  </si>
+  <si>
+    <t>Week46</t>
+  </si>
+  <si>
+    <t>Week45</t>
+  </si>
+  <si>
+    <t>Week44</t>
+  </si>
+  <si>
+    <t>Week43</t>
+  </si>
+  <si>
+    <t>Week42</t>
+  </si>
+  <si>
+    <t>Week41</t>
+  </si>
+  <si>
+    <t>Week40</t>
+  </si>
+  <si>
+    <t>Week39</t>
+  </si>
+  <si>
+    <t>Week38</t>
+  </si>
+  <si>
+    <t>Week37</t>
   </si>
 </sst>
 </file>
@@ -880,7 +920,27 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -948,6 +1008,36 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1304,8 +1394,8 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1334,22 +1424,22 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <f>SUM(C3:C4)</f>
         <v>4</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <f>SUM(D3:D4)</f>
         <v>4</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <f>D2/C2</f>
         <v>1</v>
       </c>
@@ -1390,24 +1480,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <f>SUM(C6:C9)</f>
         <v>12</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="3">
         <f>SUM(D6:D9)</f>
-        <v>11</v>
-      </c>
-      <c r="E5" s="5">
-        <f t="shared" si="0"/>
-        <v>0.91666666666666663</v>
+        <v>12</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1457,11 +1547,11 @@
         <v>3</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -1482,24 +1572,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <f>SUM(C11,C13,C14,C15,C17,C18,C19,C21,C22,C24,C25,C26,C27,C28)</f>
         <v>31</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <f>SUM(D11,D13,D14,D15,D17,D18,D19,D21,D22,D24,D25,D26,D27,D28)</f>
-        <v>1</v>
-      </c>
-      <c r="E10" s="5">
-        <f t="shared" si="0"/>
-        <v>3.2258064516129031E-2</v>
+        <v>5</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.16129032258064516</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1520,22 +1610,22 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1">
+    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
         <v>3.2</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <f>SUM(C13:C15)</f>
         <v>4</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <f>SUM(D13:D15)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1585,22 +1675,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
+    <row r="16" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
         <v>3.3</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <f>SUM(C17:C19)</f>
         <v>6</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <f>SUM(D17:D19)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1650,22 +1740,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1">
+    <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="2">
         <v>3.4</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <f>SUM(C21:C22)</f>
         <v>4</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <f>SUM(D21:D22)</f>
         <v>0</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1700,24 +1790,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
+    <row r="23" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="2">
         <v>3.5</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <f>SUM(C24:C26)</f>
         <v>5</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <f>SUM(D24:D26)</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1730,9 +1820,12 @@
       <c r="C24">
         <v>1</v>
       </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
       <c r="E24" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1745,9 +1838,12 @@
       <c r="C25">
         <v>2</v>
       </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
       <c r="E25" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1760,9 +1856,12 @@
       <c r="C26">
         <v>2</v>
       </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
       <c r="E26" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1795,24 +1894,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
+    <row r="29" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
         <v>4</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="3">
         <f>SUM(C30:C39)</f>
         <v>21</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="3">
         <f>SUM(D30:D39)</f>
-        <v>0</v>
-      </c>
-      <c r="E29" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="E29" s="4">
+        <f t="shared" si="0"/>
+        <v>9.5238095238095233E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1825,9 +1924,12 @@
       <c r="C30">
         <v>1</v>
       </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
       <c r="E30" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1870,9 +1972,12 @@
       <c r="C33">
         <v>4</v>
       </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
       <c r="E33" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -1965,22 +2070,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="1">
+    <row r="40" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
         <v>5</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="3">
         <f>SUM(C41:C46)</f>
         <v>10</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="3">
         <f>SUM(D41:D46)</f>
         <v>0</v>
       </c>
-      <c r="E40" s="5">
+      <c r="E40" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2075,22 +2180,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="1">
+    <row r="47" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="2">
         <v>6</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="3">
         <f>SUM(C48:C53)</f>
         <v>18</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="3">
         <f>SUM(D48:D53)</f>
         <v>0</v>
       </c>
-      <c r="E47" s="5">
+      <c r="E47" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2185,21 +2290,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B54" t="s">
+    <row r="54" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="2"/>
+      <c r="B54" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="3">
         <f>SUM(C2,C5,C10,C29,C40,C47)</f>
         <v>96</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="3">
         <f>SUM(D2,D5,D10,D29,D40,D47)</f>
-        <v>16</v>
-      </c>
-      <c r="E54" s="5">
-        <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>23</v>
+      </c>
+      <c r="E54" s="4">
+        <f t="shared" si="0"/>
+        <v>0.23958333333333334</v>
       </c>
     </row>
   </sheetData>
@@ -3452,19 +3558,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:Q54">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:Q55">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="between">
       <formula>6</formula>
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="lessThan">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3479,7 +3585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D284DF7B-1DF5-4BA6-BB5F-53F88794F0DA}">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J39" sqref="J39"/>
     </sheetView>
@@ -4323,12 +4429,15 @@
       <c r="D39" s="1">
         <v>4.9000000000000004</v>
       </c>
+      <c r="J39">
+        <v>2</v>
+      </c>
       <c r="L39">
         <v>1</v>
       </c>
       <c r="R39" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S39" s="5"/>
     </row>
@@ -4674,7 +4783,7 @@
       </c>
       <c r="J55">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K55">
         <f t="shared" si="1"/>
@@ -4706,27 +4815,1293 @@
       </c>
       <c r="R55" s="7">
         <f>SUM(E55:Q55)</f>
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:Q54">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:Q55">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="between">
       <formula>6</formula>
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A11409-B432-4588-B788-E05D1B49D019}">
+  <dimension ref="A1:S55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K33" sqref="K33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="42.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7265625" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="S1" s="4"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="5"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="R3" s="7">
+        <f t="shared" ref="R3:R54" si="0">SUM(E3:Q3)</f>
+        <v>2</v>
+      </c>
+      <c r="S3" s="5"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="R4" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S4" s="5"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="S5" s="5"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="R6" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="S6" s="5"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="R7" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="S7" s="5"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="R8" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="S8" s="5"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="R9" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="S9" s="5"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="S10" s="5"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="R11" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S11" s="5"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="S12" s="5"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3.2</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="R13" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S13" s="5"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="R14" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S14" s="5"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="R15" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S15" s="5"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="S16" s="5"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+      <c r="R17" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S17" s="5"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+      <c r="R18" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S18" s="5"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="R19" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S19" s="5"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S20" s="5"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="R21" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S21" s="5"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L22">
+        <v>3</v>
+      </c>
+      <c r="R22" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="S22" s="5"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="S23" s="5"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="R24" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S24" s="5"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="R25" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S25" s="5"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="R26" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S26" s="5"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L27">
+        <v>5</v>
+      </c>
+      <c r="R27" s="7">
+        <f>SUM(E27:Q27)</f>
+        <v>5</v>
+      </c>
+      <c r="S27" s="5"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A28" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="O28">
+        <v>5</v>
+      </c>
+      <c r="R28" s="7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="S28" s="5"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A29" s="1">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" t="s">
+        <v>60</v>
+      </c>
+      <c r="S29" s="5"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A30" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="R30" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S30" s="5"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A31" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="M31">
+        <v>3</v>
+      </c>
+      <c r="R31" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="S31" s="5"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="M32">
+        <v>3</v>
+      </c>
+      <c r="R32" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="S32" s="5"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>3</v>
+      </c>
+      <c r="R33" s="7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="S33" s="5"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A34" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J34">
+        <v>3</v>
+      </c>
+      <c r="R34" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="S34" s="5"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>60</v>
+      </c>
+      <c r="D35" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="J35">
+        <v>1</v>
+      </c>
+      <c r="R35" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S35" s="5"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A36" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="R36" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S36" s="5"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A37" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="R37" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S37" s="5"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="B38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M38">
+        <v>2</v>
+      </c>
+      <c r="R38" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S38" s="5"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" t="s">
+        <v>71</v>
+      </c>
+      <c r="C39" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" s="1">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="R39" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S39" s="5"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A40" s="1">
+        <v>5</v>
+      </c>
+      <c r="B40" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="S40" s="5"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A41" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B41" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N41">
+        <v>2</v>
+      </c>
+      <c r="R41" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S41" s="5"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="R42" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S42" s="5"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="N43">
+        <v>2</v>
+      </c>
+      <c r="R43" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S43" s="5"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" t="s">
+        <v>58</v>
+      </c>
+      <c r="D44" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+      <c r="R44" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S44" s="5"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A45" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="B45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" t="s">
+        <v>58</v>
+      </c>
+      <c r="D45" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="O45">
+        <v>2</v>
+      </c>
+      <c r="R45" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S45" s="5"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="O46">
+        <v>2</v>
+      </c>
+      <c r="R46" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S46" s="5"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="S47" s="5"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A48" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="P48">
+        <v>2</v>
+      </c>
+      <c r="R48" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S48" s="5"/>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="P49">
+        <v>2</v>
+      </c>
+      <c r="R49" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S49" s="5"/>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="B50" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="P50">
+        <v>2</v>
+      </c>
+      <c r="R50" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S50" s="5"/>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A51" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="B51" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="Q51">
+        <v>2</v>
+      </c>
+      <c r="R51" s="7">
+        <f>SUM(E51:Q51)</f>
+        <v>2</v>
+      </c>
+      <c r="S51" s="5"/>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q52">
+        <v>4</v>
+      </c>
+      <c r="R52" s="7">
+        <f>SUM(E52:Q52)</f>
+        <v>4</v>
+      </c>
+      <c r="S52" s="5"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>6.6</v>
+      </c>
+      <c r="B53" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="P53">
+        <v>6</v>
+      </c>
+      <c r="R53" s="7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="S53" s="5"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" t="s">
+        <v>91</v>
+      </c>
+      <c r="C54" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="P54">
+        <v>1</v>
+      </c>
+      <c r="R54" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S54" s="5"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="D55" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E55">
+        <f>SUM(E2:E54)</f>
+        <v>5</v>
+      </c>
+      <c r="F55">
+        <f t="shared" ref="F55:Q55" si="1">SUM(F2:F54)</f>
+        <v>7</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L55">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="R55" s="7">
+        <f>SUM(E55:Q55)</f>
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2:Q12 E53:Q54 E51:O52 Q51:Q52 E48:N49 P48:Q49 E47:Q47 E45:M46 O45:Q46 E41:L44 N41:Q44 E50:M50 O50:Q50 E27:Q30 E13:I16 E17:H19 L25:Q26 E20:I26 E31:J35 E40:Q40 E36:K39 M34:Q39 L33:Q33 M31:Q32 K13:Q20 K23:Q24 L21:Q22">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55:Q55">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="between">
+      <formula>6</formula>
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
+      <formula>6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="greaterThan">
+      <formula>9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J25">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J26">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated wbs and pop to reflect how I actually plan to work
</commit_message>
<xml_diff>
--- a/wbs-and-pop.xlsx
+++ b/wbs-and-pop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ander\work\H25\konstruksjon-av-innebygde-systemer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490E0718-FA40-4B25-8E49-A4D2D819BD9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D677852-D06C-473F-92D7-2B565FAF7E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" activeTab="3" xr2:uid="{88374655-B4FF-47ED-8C62-5C3447431953}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{88374655-B4FF-47ED-8C62-5C3447431953}"/>
   </bookViews>
   <sheets>
     <sheet name="work-breakdown-structure" sheetId="2" r:id="rId1"/>
@@ -920,17 +920,7 @@
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -1393,9 +1383,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61304A7E-7105-49C5-87C3-17E3D711999C}">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1585,11 +1575,11 @@
       </c>
       <c r="D10" s="3">
         <f>SUM(D11,D13,D14,D15,D17,D18,D19,D21,D22,D24,D25,D26,D27,D28)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>0.16129032258064516</v>
+        <v>6.4516129032258063E-2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -1803,11 +1793,11 @@
       </c>
       <c r="D23" s="3">
         <f>SUM(D24:D26)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1838,12 +1828,9 @@
       <c r="C25">
         <v>2</v>
       </c>
-      <c r="D25">
-        <v>2</v>
-      </c>
       <c r="E25" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1856,12 +1843,9 @@
       <c r="C26">
         <v>2</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
       <c r="E26" s="5">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1907,11 +1891,11 @@
       </c>
       <c r="D29" s="3">
         <f>SUM(D30:D39)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="4">
         <f t="shared" si="0"/>
-        <v>9.5238095238095233E-2</v>
+        <v>4.7619047619047616E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1972,12 +1956,9 @@
       <c r="C33">
         <v>4</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
       <c r="E33" s="5">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -2301,11 +2282,11 @@
       </c>
       <c r="D54" s="3">
         <f>SUM(D2,D5,D10,D29,D40,D47)</f>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E54" s="4">
         <f t="shared" si="0"/>
-        <v>0.23958333333333334</v>
+        <v>0.19791666666666666</v>
       </c>
     </row>
   </sheetData>
@@ -3558,19 +3539,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:Q54">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:Q55">
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="between">
       <formula>6</formula>
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="lessThan">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4820,19 +4801,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:Q54">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:Q55">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
       <formula>6</formula>
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4844,9 +4825,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A11409-B432-4588-B788-E05D1B49D019}">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K33" sqref="K33"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5141,7 +5122,7 @@
       <c r="D13" s="1">
         <v>3.2</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>2</v>
       </c>
       <c r="R13" s="7">
@@ -5163,7 +5144,7 @@
       <c r="D14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>1</v>
       </c>
       <c r="R14" s="7">
@@ -5185,7 +5166,7 @@
       <c r="D15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>1</v>
       </c>
       <c r="R15" s="7">
@@ -5222,7 +5203,7 @@
       <c r="D17" s="1">
         <v>3.3</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>2</v>
       </c>
       <c r="R17" s="7">
@@ -5244,7 +5225,7 @@
       <c r="D18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>2</v>
       </c>
       <c r="R18" s="7">
@@ -5266,7 +5247,7 @@
       <c r="D19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>2</v>
       </c>
       <c r="R19" s="7">
@@ -5384,7 +5365,7 @@
       <c r="D25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I25">
+      <c r="L25">
         <v>2</v>
       </c>
       <c r="R25" s="7">
@@ -5406,11 +5387,8 @@
       <c r="D26" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-      <c r="J26">
-        <v>1</v>
+      <c r="L26">
+        <v>2</v>
       </c>
       <c r="R26" s="7">
         <f t="shared" si="0"/>
@@ -5432,7 +5410,10 @@
         <v>54</v>
       </c>
       <c r="L27">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="M27">
+        <v>3</v>
       </c>
       <c r="R27" s="7">
         <f>SUM(E27:Q27)</f>
@@ -5556,7 +5537,7 @@
       <c r="I33">
         <v>1</v>
       </c>
-      <c r="J33">
+      <c r="M33">
         <v>3</v>
       </c>
       <c r="R33" s="7">
@@ -5578,7 +5559,7 @@
       <c r="D34" s="1">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J34">
+      <c r="M34">
         <v>3</v>
       </c>
       <c r="R34" s="7">
@@ -5600,7 +5581,7 @@
       <c r="D35" s="1">
         <v>4.5</v>
       </c>
-      <c r="J35">
+      <c r="M35">
         <v>1</v>
       </c>
       <c r="R35" s="7">
@@ -5688,7 +5669,7 @@
       <c r="D39" s="1">
         <v>4.9000000000000004</v>
       </c>
-      <c r="M39">
+      <c r="N39">
         <v>1</v>
       </c>
       <c r="R39" s="7">
@@ -5813,7 +5794,7 @@
       <c r="D45" s="1">
         <v>5.4</v>
       </c>
-      <c r="O45">
+      <c r="N45">
         <v>2</v>
       </c>
       <c r="R45" s="7">
@@ -5835,7 +5816,7 @@
       <c r="D46" s="1">
         <v>5.5</v>
       </c>
-      <c r="O46">
+      <c r="N46">
         <v>2</v>
       </c>
       <c r="R46" s="7">
@@ -5872,7 +5853,7 @@
       <c r="D48" s="1">
         <v>5.6</v>
       </c>
-      <c r="P48">
+      <c r="O48">
         <v>2</v>
       </c>
       <c r="R48" s="7">
@@ -5894,7 +5875,7 @@
       <c r="D49" s="1">
         <v>6.1</v>
       </c>
-      <c r="P49">
+      <c r="O49">
         <v>2</v>
       </c>
       <c r="R49" s="7">
@@ -5916,7 +5897,7 @@
       <c r="D50" s="1">
         <v>6.1</v>
       </c>
-      <c r="P50">
+      <c r="O50">
         <v>2</v>
       </c>
       <c r="R50" s="7">
@@ -6035,35 +6016,35 @@
       </c>
       <c r="I55">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J55">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="K55">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L55">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="M55">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="N55">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="O55">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="P55">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="Q55">
         <f t="shared" si="1"/>
@@ -6075,29 +6056,24 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:Q12 E53:Q54 E51:O52 Q51:Q52 E48:N49 P48:Q49 E47:Q47 E45:M46 O45:Q46 E41:L44 N41:Q44 E50:M50 O50:Q50 E27:Q30 E13:I16 E17:H19 L25:Q26 E20:I26 E31:J35 E40:Q40 E36:K39 M34:Q39 L33:Q33 M31:Q32 K13:Q20 K23:Q24 L21:Q22">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="E2:Q12 E13:I16 L13:L19 N13:Q19 E17:H19 K20:Q20 E20:I26 L21:Q22 K23:Q24 E27:Q30 E31:J32 M31:Q32 L33:Q33 E33:I35 M33:M35 M34:Q38 E36:K39 N39:Q39 E40:Q40 E41:L44 N41:Q44 E45:N46 P45:Q46 E47:Q47 E48:N49 O48:O50 Q48:Q52 E50:M50 E51:O52 E53:Q54">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:Q55">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="between">
       <formula>6</formula>
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="lessThan">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J25">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J26">
+  <conditionalFormatting sqref="L25:Q26">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>